<commit_message>
Basics of periodic analysis working
</commit_message>
<xml_diff>
--- a/code/example_periodic.xlsx
+++ b/code/example_periodic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cr591_exeter_ac_uk/Documents/Desktop/PhD/Projects/diametrics-webapp-dash/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8A6BCDD-4C8A-4DAD-A347-C82D9B8BF3AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{D8A6BCDD-4C8A-4DAD-A347-C82D9B8BF3AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD3182DA-647A-438C-B494-65F8E6CC5232}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{0CE94312-C88D-499E-AA40-48D198AB2435}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CE94312-C88D-499E-AA40-48D198AB2435}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>startDateTime</t>
-  </si>
-  <si>
-    <t>endDateTime</t>
-  </si>
-  <si>
     <t>1006_baseline</t>
   </si>
   <si>
@@ -54,6 +48,12 @@
   </si>
   <si>
     <t>Meal</t>
+  </si>
+  <si>
+    <t>endDatetime</t>
+  </si>
+  <si>
+    <t>startDatetime</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,18 +465,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>43110.75</v>
@@ -485,12 +485,12 @@
         <v>43110.8125</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>43112.791666666664</v>
@@ -499,12 +499,12 @@
         <v>43112.833333333336</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2">
         <v>43115.416666666664</v>
@@ -513,12 +513,12 @@
         <v>43115.5</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2">
         <v>43116.458333333336</v>
@@ -527,12 +527,12 @@
         <v>43116.489583333336</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2">
         <v>43110.375</v>
@@ -541,12 +541,12 @@
         <v>43110.395833333336</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2">
         <v>43111.375</v>
@@ -555,12 +555,12 @@
         <v>43111.395833333336</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2">
         <v>43112.375</v>
@@ -569,12 +569,12 @@
         <v>43112.395833333336</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2">
         <v>43113.375</v>
@@ -583,12 +583,12 @@
         <v>43113.395833333336</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" s="2">
         <v>43114.375</v>
@@ -597,12 +597,12 @@
         <v>43114.395833333336</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2">
         <v>43115.375</v>
@@ -611,12 +611,12 @@
         <v>43115.395833333336</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2">
         <v>43116.375</v>
@@ -625,12 +625,12 @@
         <v>43116.395833333336</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" s="2">
         <v>43110.541666608799</v>
@@ -639,12 +639,12 @@
         <v>43110.5625</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2">
         <v>43111.541666608799</v>
@@ -653,12 +653,12 @@
         <v>43111.5625</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" s="2">
         <v>43112.541666608799</v>
@@ -667,12 +667,12 @@
         <v>43112.5625</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16" s="2">
         <v>43113.541666608799</v>
@@ -681,12 +681,12 @@
         <v>43113.5625</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" s="2">
         <v>43114.541666608799</v>
@@ -695,12 +695,12 @@
         <v>43114.5625</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B18" s="2">
         <v>43115.541666608799</v>
@@ -709,12 +709,12 @@
         <v>43115.5625</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B19" s="2">
         <v>43116.541666608799</v>
@@ -723,12 +723,12 @@
         <v>43116.5625</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20" s="2">
         <v>43110.8125</v>
@@ -737,12 +737,12 @@
         <v>43110.854166608799</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21" s="2">
         <v>43111.8125</v>
@@ -751,12 +751,12 @@
         <v>43111.854166608799</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B22" s="2">
         <v>43112.8125</v>
@@ -765,12 +765,12 @@
         <v>43112.854166608799</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B23" s="2">
         <v>43113.8125</v>
@@ -779,12 +779,12 @@
         <v>43113.854166608799</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B24" s="2">
         <v>43114.8125</v>
@@ -793,12 +793,12 @@
         <v>43114.854166608799</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B25" s="2">
         <v>43115.8125</v>
@@ -807,7 +807,7 @@
         <v>43115.854166608799</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -816,6 +816,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006088DFC06585324090D8E4894142CCE5" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60bfbe0c8909a620725064eab651d69f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dfa44a58-9fb3-4433-a208-2627b51d74d1" xmlns:ns4="74adf222-4ff3-4e51-967f-f17228447fcb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="32d11ee019eb494ed63df5a75d0970e1" ns3:_="" ns4:_="">
     <xsd:import namespace="dfa44a58-9fb3-4433-a208-2627b51d74d1"/>
@@ -1044,22 +1059,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{311861A7-52A8-4817-AC7D-426C0BED9D57}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33FB9C4C-7A43-4FD4-BEC5-1D1DAD669BBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96DECC97-B17C-4AAA-A607-2415BA1CD723}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1076,21 +1093,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33FB9C4C-7A43-4FD4-BEC5-1D1DAD669BBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{311861A7-52A8-4817-AC7D-426C0BED9D57}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>